<commit_message>
Add Contract completed / start on vendor list cleanup
</commit_message>
<xml_diff>
--- a/Contract_WIP.xlsx
+++ b/Contract_WIP.xlsx
@@ -1,37 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-28920" yWindow="-1470"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,24 +43,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -330,13 +317,133 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="13.7109375"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="9.85546875"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="13.42578125"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" width="10.28515625"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" width="13.42578125"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" width="4.42578125"/>
+    <col bestFit="1" customWidth="1" max="9" min="9" width="20"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Date Awarded</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Contract #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Qty</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Contract Total</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>NSN</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Part Name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Vendor Name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>P/N</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Preservation Method</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Due Date</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>3/5/2019</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>4654</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>654</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>464</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>65464</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>4654</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>654</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>654</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
connect main sheet to PO creation
</commit_message>
<xml_diff>
--- a/Contract_WIP.xlsx
+++ b/Contract_WIP.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-28920" yWindow="-1470"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="13140" windowWidth="24240" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -323,13 +323,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="13.7109375"/>
     <col bestFit="1" customWidth="1" max="2" min="2" width="17.7109375"/>
@@ -339,8 +339,7 @@
     <col bestFit="1" customWidth="1" max="6" min="6" width="38"/>
     <col bestFit="1" customWidth="1" max="7" min="7" width="13.42578125"/>
     <col bestFit="1" customWidth="1" max="8" min="8" width="18.140625"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" width="20"/>
-    <col bestFit="1" customWidth="1" max="11" min="10" width="11.7109375"/>
+    <col bestFit="1" customWidth="1" max="10" min="9" width="11.7109375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -386,15 +385,10 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Unit Price</t>
+          <t>Preservation Method</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
-        <is>
-          <t>Preservation Method</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
         <is>
           <t>Due Date</t>
         </is>
@@ -439,12 +433,12 @@
           <t>319HA112NFP25DN</t>
         </is>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr">
-        <is>
-          <t>CP</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
         <is>
           <t>2019 AUG 26</t>
         </is>
@@ -489,12 +483,12 @@
           <t>497-0756</t>
         </is>
       </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
       <c r="J3" t="inlineStr">
-        <is>
-          <t>CP</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
         <is>
           <t>2019 AUG 26</t>
         </is>
@@ -539,12 +533,12 @@
           <t>ADTS405189433M0</t>
         </is>
       </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr">
-        <is>
-          <t>CP</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
         <is>
           <t>2019 AUG 26</t>
         </is>
@@ -589,12 +583,12 @@
           <t>479033</t>
         </is>
       </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
       <c r="J5" t="inlineStr">
-        <is>
-          <t>CP</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
         <is>
           <t>2019 AUG 26</t>
         </is>
@@ -639,12 +633,12 @@
           <t>822901</t>
         </is>
       </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
       <c r="J6" t="inlineStr">
-        <is>
-          <t>CP</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
         <is>
           <t>2019 AUG 26</t>
         </is>
@@ -689,12 +683,12 @@
           <t>144392</t>
         </is>
       </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
       <c r="J7" t="inlineStr">
-        <is>
-          <t>CP</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
         <is>
           <t>2019 SEP 16</t>
         </is>
@@ -739,12 +733,12 @@
           <t>TPV66345-1002</t>
         </is>
       </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
       <c r="J8" t="inlineStr">
-        <is>
-          <t>CP</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
         <is>
           <t>2019 OCT 20</t>
         </is>
@@ -793,15 +787,10 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>664.00</t>
+          <t>M41</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
-        <is>
-          <t>41</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
         <is>
           <t>2019 JUL 18</t>
         </is>
@@ -850,15 +839,10 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>4,787.00</t>
+          <t>CP</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
-        <is>
-          <t>CP</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
         <is>
           <t>2019 AUG 27</t>
         </is>
@@ -907,15 +891,10 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>2,317.00</t>
+          <t>CP</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
-        <is>
-          <t>CP</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
         <is>
           <t>2019 SEP 16</t>
         </is>
@@ -964,15 +943,10 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>574.60</t>
+          <t>CP</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
-        <is>
-          <t>CP</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
         <is>
           <t>2019 AUG 22</t>
         </is>
@@ -1021,15 +995,10 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>1,038.81</t>
+          <t>CP</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
-        <is>
-          <t>CP</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
         <is>
           <t>2019 AUG 28</t>
         </is>
@@ -1078,15 +1047,10 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>8,289.00</t>
+          <t>CP</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
-        <is>
-          <t>CP</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
         <is>
           <t>2019 SEP 17</t>
         </is>
@@ -1135,17 +1099,324 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>28.63</t>
+          <t>M10</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
           <t>2019 JUL 22</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>3/25/2019</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SPE7M2-19-V-1046</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>$32,557.65</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>5330010778314</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>PACKING ASSORTMENT,PREFORMED</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Munters</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>43125-08</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>M33</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>2019 SEP 03</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>3/25/2019</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SPE7L1-19-V-4818</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>$2,224.00</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>3020016570251</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>GEAR,ANTIBACKLASH,H</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>KTSDI</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>510251-163</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>M41</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>2019 JUN 28</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>3/25/2019</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SPE7M0-19-V-6074</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>$12,650.22</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>5930013674492</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>SWITCH,FLOW</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>GEMS</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>139644</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>2019 SEP 03</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>3/25/2019</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>SPE7M0-19-V-6059</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>$6,219.84</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>5930014842487</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>SWITCH,FLOW</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>GEMS</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>159297</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>2019 SEP 03</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>3/25/2019</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SPE7MC-19-V-5914</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>$4,654.00 </t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>5935014967270</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>BACKSHELL,ELECTRICAL CONNECTOR</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>447HT325XW2519</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>2019 SEP 03</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>3/25/2019</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SPE7M1-19-V-5446</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>$9,545.28 </t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>6110014091404</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>CONTROLLER,MOTOR</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Morpac</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>70000-4</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>2019 SEP 03</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Email password hiding / PO Email complete
</commit_message>
<xml_diff>
--- a/Contract_WIP.xlsx
+++ b/Contract_WIP.xlsx
@@ -323,7 +323,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
@@ -1576,6 +1576,162 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>3/27/2019</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>SPE7M1-19-V-5560</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>$7,011.31</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>5998016130768</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>CIRCUIT CARD ASSEMBLY</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>DIT-MCO</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>114-02254-0003</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>GX</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>2019 AUG 14</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>3/27/2019</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>SPE7MC-19-V-6036</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>$3,085.52</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>4820011455601</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>DISK,VALVE</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Griswold</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>39983C</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>2019 SEP 03</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>3/27/2019</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>SPE7MC-19-V-6070</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>$4,944.30</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>5935015103860</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>BACKSHELL,ELECTRICAL CONNECTOR</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>440BJ031NF2710N</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>2019 SEP 03</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Attempted PO feature addition / bug fixes
</commit_message>
<xml_diff>
--- a/Contract_WIP.xlsx
+++ b/Contract_WIP.xlsx
@@ -323,13 +323,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="13.7109375"/>
     <col bestFit="1" customWidth="1" max="2" min="2" width="17.7109375"/>
@@ -1836,6 +1836,162 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>4/1/2019</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>SPE7M5-19-V-7228</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>$629.00</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>5935015527394</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>BACKSHELL,ELECTRICAL CONNECTOR</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>390AS002NF0804H3</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>2019 SEP 09</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>4/1/2019</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>SPE4A6-19-V-070V</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>$17,032.68</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>5342015037327</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>MAGNET,HOLDER ASSY</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>GEMS</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>137444</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>ZZ</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>2019 SEP 09</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>4/2/2019</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>SPE7M5-19-P-6235</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>$65,145.00</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>5935016786944</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>BACKSHELL,ELECTRICAL CONNECTOR</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>445HS065NF25064</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>2019 SEP 19</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Contract Management repair bug fixed
</commit_message>
<xml_diff>
--- a/Contract_WIP.xlsx
+++ b/Contract_WIP.xlsx
@@ -323,13 +323,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="13.7109375"/>
     <col bestFit="1" customWidth="1" max="2" min="2" width="17.7109375"/>
@@ -2096,6 +2096,318 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>4/4/2019</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>654</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>654</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>654</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>654</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>654</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>654</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>654</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>654</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>654</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>4/4/2019</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>6987</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>9456</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>453</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>15849</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>489</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>4968</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>484</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>4/4/2019</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>984</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>65156</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>484</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>415</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>684894</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>4/4/2019</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>654</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>878</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>7979</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>8798</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>7987</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>4/4/2019</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>897</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>987</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>7798</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>798</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>7987</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>4/4/2019</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>654</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>564</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>6456</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>564</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>56465</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>456</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>4654</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Inventory window creation / logic planned out
</commit_message>
<xml_diff>
--- a/Contract_WIP.xlsx
+++ b/Contract_WIP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Avinash Patel\Desktop\WestSim_App\WestSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2247C1-7038-48E3-9E1A-190121F452BE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E747FB-8D5B-47D2-A7DF-47DF150B0FF3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1579,8 +1579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1592,7 +1592,7 @@
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Inventory Add functionality finished
</commit_message>
<xml_diff>
--- a/Contract_WIP.xlsx
+++ b/Contract_WIP.xlsx
@@ -323,7 +323,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J91"/>
+  <dimension ref="A1:J95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="H41" sqref="H41"/>
@@ -5061,6 +5061,214 @@
         </is>
       </c>
     </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>4/18/2019</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>SPE5EM-19-V-4069</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>$299.94 </t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>5330016570078</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>SEAL,PLAIN</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>KTSDI</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>180X210L08N</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>M33</t>
+        </is>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>2019 AUG 16</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>4/18/2019</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>SPE7M5-19-V-8001</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>125</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>$745.00</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>5920015723699</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>FUSE,CARTRIDGE</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Rohde Schwarz</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>0099-6729-00</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>2019 AUG 16</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>4/18/2019</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>SPE7M2-19-V-1181</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>$769.44 </t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>5355011119493</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>POINTER,DIAL</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Cameron</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>0315-0005.B</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>M30</t>
+        </is>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>2019 SEP 05</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>4/19/2019</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>SPE7MC-19-V-7094</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>$4,609.86 </t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>5915015956493</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>FILTER,RADIO FREQUE</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Genisco</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>GF68200-50B</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>2019 OCT 07</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Inventory search function mostly done, edit function next
</commit_message>
<xml_diff>
--- a/Contract_WIP.xlsx
+++ b/Contract_WIP.xlsx
@@ -323,7 +323,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J100"/>
+  <dimension ref="A1:J102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="H41" sqref="H41"/>
@@ -5529,6 +5529,110 @@
         </is>
       </c>
     </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>4/23/2019</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>SPE4A4-19-V-5882</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>$6,637.10</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>6680010876055</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>TRANSMITTER,LIQUID</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>GEMS</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>48098</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>ZZ</t>
+        </is>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>2019 SEP 30</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>4/23/2019</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>SPE7L3-19-V-5652</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>$1,679.36 </t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>3040012589487</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>PLATE,RETAINING,SHA</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>Timken</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>2051G92-001</t>
+        </is>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>2019 SEP 30</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Inventory Edit functionaly finished
</commit_message>
<xml_diff>
--- a/Contract_WIP.xlsx
+++ b/Contract_WIP.xlsx
@@ -323,7 +323,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J102"/>
+  <dimension ref="A1:J105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="H41" sqref="H41"/>
@@ -5633,6 +5633,162 @@
         </is>
       </c>
     </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>4/24/2019</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>SPE7L4-19-V-0874</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>$2,389.38 </t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>5935012860663</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>CONNECTOR,PLUG,ELEC</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>ITT</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>CIR06G2-14S-6S-F80</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>ZZ</t>
+        </is>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>2019 OCT 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>4/24/2019</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>SPE8E8-19-V-1727</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>$5,114.82</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>4420015045491</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>BAFFLE,FLUID COOLER</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>Fluid Handling</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>4371641-0476</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>2019 OCT 01</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>4/24/2019</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>SPE7M1-19-V-6499</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>$1,677.39 </t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>5999012232712</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>DELAY LINE</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>Data Delay Devices</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>DDU7-8212</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>2019 OCT 01</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Weekend catch-up / tbd empty row fix
</commit_message>
<xml_diff>
--- a/Contract_WIP.xlsx
+++ b/Contract_WIP.xlsx
@@ -323,7 +323,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J105"/>
+  <dimension ref="A1:J109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="H41" sqref="H41"/>
@@ -5789,6 +5789,214 @@
         </is>
       </c>
     </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>4/25/2019</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>SPE5EM-19-V-4186</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>$324.00 </t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>5330012549189</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>GASKET</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>American Metal Bearing</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>G001</t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>M33</t>
+        </is>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>2019 OCT 02</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>4/26/2019</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>SPE4A6-19-P-E296</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>$13,695.42</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>5895016527348</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>TRANSMITTER GROUP</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>GEMS</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>822610</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>M41</t>
+        </is>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>2019 OCT 07</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>4/26/2019</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>SPE7M8-19-P-2323</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>$16,436.00</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>5930014065242</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>SWITCH,LIQUID LEVEL</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>GEMS</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>LS-76725</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>2019 OCT 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>4/26/2019</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>SPE4A6-19-V-136J</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>$61,583.70 </t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>6680013650925</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>TRANSMITTER,LIQUID</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>GEMS</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>42880-0105</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>2019 OCT 08</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
New month cleanup / inventory additions
</commit_message>
<xml_diff>
--- a/Contract_WIP.xlsx
+++ b/Contract_WIP.xlsx
@@ -323,7 +323,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J112"/>
+  <dimension ref="A1:J116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="H41" sqref="H41"/>
@@ -6153,6 +6153,214 @@
         </is>
       </c>
     </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>4/30/2019</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>SPE7L0-19-V-5061</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>$7,539.00 </t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>6130014243614</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>POWER SUPPLY</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>GEMS</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>144875</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>2019 OCT 07</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>4/30/2019</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>SPE7MC-19-V-7482</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>$4,344.00</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>5935014489052</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>BACKSHELL,ELECTRICA</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>712FS277NF1012-31</t>
+        </is>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>2019 OCT 07</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>4/30/2019</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>SPE5E3-19-V-7870</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>$391.14 </t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>5330013722277</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>GASKET</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>Timken</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>01070-0279LOC6-11</t>
+        </is>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>M33</t>
+        </is>
+      </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>2019 OCT 07</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>4/30/2019</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>SPE5E3-19-V-7833</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>$391.41</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>5330013722276</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>GASKET</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>Timken</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>01070-0279LOC6-9</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>M33</t>
+        </is>
+      </c>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t>2019 OCT 07</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
package catch up / WAWF planning
</commit_message>
<xml_diff>
--- a/Contract_WIP.xlsx
+++ b/Contract_WIP.xlsx
@@ -45,10 +45,13 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -324,10 +327,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J156"/>
+  <dimension ref="A1:J172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="D148" sqref="D148"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -8096,7 +8099,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>$17,991.62 </t>
+          <t>$17,991.62</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
@@ -8200,7 +8203,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>$390.88 </t>
+          <t>$390.88</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
@@ -8252,7 +8255,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>$35,473.96 </t>
+          <t>$35,473.96</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
@@ -8391,10 +8394,8 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" t="inlineStr">
-        <is>
-          <t>5/21/2019</t>
-        </is>
+      <c r="A156" s="3" t="n">
+        <v>43607</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
@@ -8439,6 +8440,838 @@
       <c r="J156" t="inlineStr">
         <is>
           <t>2019 OCT 28</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>5/22/2019</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>SPE7M1-19-V-7384</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>$7,505.30</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>5935015998509</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>CLAMP,CABLE,ELECTRI</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>319HB105NF15DN</t>
+        </is>
+      </c>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J157" t="inlineStr">
+        <is>
+          <t>2019 NOV 08</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>5/22/2019</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>SPE7M1-19-V-7371</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>$3,070.76</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>5998015867425</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>CIRCUIT CARD ASSEMB</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>FCX</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>AMA738000</t>
+        </is>
+      </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>GX</t>
+        </is>
+      </c>
+      <c r="J158" t="inlineStr">
+        <is>
+          <t>2019 OCT 29</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>5/22/2019</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>SPE7M5-19-V-9185</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>$3,635.40</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>5935014597025</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>BACKSHELL,DUMMY CON</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>370HS001NF1108H4</t>
+        </is>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J159" t="inlineStr">
+        <is>
+          <t>2019 NOV 18</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>5/22/2019</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>SPE7M1-19-V-7260</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>$2,675.85</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>5935016151707</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>BACKSHELL,ELECTRICA</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>447HW325XW1913B</t>
+        </is>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J160" t="inlineStr">
+        <is>
+          <t>2019 NOV 18</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>5/22/2019</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>SPE7M5-19-V-9205</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>$1,161.28</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>5935014612332</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>BACKSHELL,ELECTRICA</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>450AA005NF14</t>
+        </is>
+      </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J161" t="inlineStr">
+        <is>
+          <t>2019 NOV 04</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>5/22/2019</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>SPE7M1-19-V-7274</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>$6,869.28</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>6110015116558</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>SLAVE POWER CONTROL</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>Indeeco</t>
+        </is>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>1020882</t>
+        </is>
+      </c>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J162" t="inlineStr">
+        <is>
+          <t>2019 OCT 29</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>5/22/2019</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>SPE7M0-19-V-7828</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>$3,983.44</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>5935016748942</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>BACKSHELL,DUMMY CON</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>390AJ001Z12416H-49A</t>
+        </is>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J163" t="inlineStr">
+        <is>
+          <t>2019 NOV 08</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>5/22/2019</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>SPE7M0-19-V-7830</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>$1,485.93 </t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>5998014355673</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>CIRCUIT CARD ASSEMBLY</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>Druck</t>
+        </is>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>ADTS405-26-1892-M0</t>
+        </is>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>GX</t>
+        </is>
+      </c>
+      <c r="J164" t="inlineStr">
+        <is>
+          <t>2019 OCT 29</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>5/23/2019</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>SPE4A6-19-V-204D</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>$2,452.75</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>5975015596748</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>ADAPTER,ELECTRICAL</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>712FS178B1428-31</t>
+        </is>
+      </c>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J165" t="inlineStr">
+        <is>
+          <t>2019 NOV 12</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>5/23/2019</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>SPE5EK-19-V-4672</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>$9,487.41</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>5340016801308</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>BRACKET,MOUNTING</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>HIAB</t>
+        </is>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>387-4832</t>
+        </is>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J166" t="inlineStr">
+        <is>
+          <t>2019 NOV 04</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>5/23/2019</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>SPE7M5-19-V-9226</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>$503.73 </t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>5945016203288</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>RELAY,SOLID STATE</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>Sauer</t>
+        </is>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>DB0008</t>
+        </is>
+      </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>M41</t>
+        </is>
+      </c>
+      <c r="J167" t="inlineStr">
+        <is>
+          <t>2019 OCT 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>5/23/2019</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>SPE4A6-19-V-203B</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>$2,500.68</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>5940016795082</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>TERMINAL BOX</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>HIAB</t>
+        </is>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>387-5300</t>
+        </is>
+      </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J168" t="inlineStr">
+        <is>
+          <t>2019 OCT 30</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>5/23/2019</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>SPE7M5-19-V-9223</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>$4,801.05 </t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>5935015998189</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>CLAMP,CABLE,ELECTRI</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>319HA112NF25DN</t>
+        </is>
+      </c>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J169" t="inlineStr">
+        <is>
+          <t>2019 NOV 12</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>5/23/2019</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>SPE7M5-19-V-9212</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>$635.84 </t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>5935013046895</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>BACKSHELL,ELECTRICA</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>Kern Engineering</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>BAT08-18W03C</t>
+        </is>
+      </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J170" t="inlineStr">
+        <is>
+          <t>2019 OCT 30</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>5/23/2019</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>SPE4A6-19-V-202Q</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>$556.00 </t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>6150013923696</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>CABLE ASSEMBLY,SPEC</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>Morpac</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>70091-2</t>
+        </is>
+      </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J171" t="inlineStr">
+        <is>
+          <t>2019 OCT 30</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>5/23/2019</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>SPE4A4-19-V-6635</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>$17,165.00 </t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>6150012081693</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>CABLE ASSEMBLY,POWE</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>GEMS</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>37890-02-10-008-HP</t>
+        </is>
+      </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J172" t="inlineStr">
+        <is>
+          <t>2019 NOV 12</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
normal day / bug detection
</commit_message>
<xml_diff>
--- a/Contract_WIP.xlsx
+++ b/Contract_WIP.xlsx
@@ -327,13 +327,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J194"/>
+  <dimension ref="A1:J196"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
       <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="13.7109375"/>
     <col bestFit="1" customWidth="1" max="2" min="2" width="17.7109375"/>
@@ -10419,6 +10419,110 @@
         </is>
       </c>
     </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>6/7/2019</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>SPE7M5-19-V-9760</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>$1,608.36</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>5935016151446</t>
+        </is>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>BACKSHELL,ELECTRICA</t>
+        </is>
+      </c>
+      <c r="G195" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H195" t="inlineStr">
+        <is>
+          <t>447HS325XW1106B</t>
+        </is>
+      </c>
+      <c r="I195" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J195" t="inlineStr">
+        <is>
+          <t>2019 NOV 25</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>6/7/2019</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>SPE7L7-19-V-1150</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>$2,394.46</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>6130014355672</t>
+        </is>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>POWER SUPPLY</t>
+        </is>
+      </c>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>Druck</t>
+        </is>
+      </c>
+      <c r="H196" t="inlineStr">
+        <is>
+          <t>ADTS405-1892-25-M0</t>
+        </is>
+      </c>
+      <c r="I196" t="inlineStr">
+        <is>
+          <t>M41</t>
+        </is>
+      </c>
+      <c r="J196" t="inlineStr">
+        <is>
+          <t>2019 NOV 14</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Email login bug fix
</commit_message>
<xml_diff>
--- a/Contract_WIP.xlsx
+++ b/Contract_WIP.xlsx
@@ -327,13 +327,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J196"/>
+  <dimension ref="A1:J197"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
       <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="13.7109375"/>
     <col bestFit="1" customWidth="1" max="2" min="2" width="17.7109375"/>
@@ -10523,6 +10523,58 @@
         </is>
       </c>
     </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>6/13/2019</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>SPE8E8-19-V-2080</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>$378.00</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>4520013773187</t>
+        </is>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>HEATING ELEMENT,ELE</t>
+        </is>
+      </c>
+      <c r="G197" t="inlineStr">
+        <is>
+          <t>Indeeco</t>
+        </is>
+      </c>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>53442</t>
+        </is>
+      </c>
+      <c r="I197" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J197" t="inlineStr">
+        <is>
+          <t>2019 NOV 20</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
po payment record function added
</commit_message>
<xml_diff>
--- a/Contract_WIP.xlsx
+++ b/Contract_WIP.xlsx
@@ -327,7 +327,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J355"/>
+  <dimension ref="A1:J357"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A271" workbookViewId="0">
       <selection activeCell="G292" sqref="G292"/>
@@ -18789,6 +18789,110 @@
         </is>
       </c>
     </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>9/13/2019</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>SPE5EK-19-V-6967</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>$187.00</t>
+        </is>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>5340015796639</t>
+        </is>
+      </c>
+      <c r="F356" t="inlineStr">
+        <is>
+          <t>COVER,PROTECTIVE,DU</t>
+        </is>
+      </c>
+      <c r="G356" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H356" t="inlineStr">
+        <is>
+          <t>660-014NF10U8-09</t>
+        </is>
+      </c>
+      <c r="I356" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J356" t="inlineStr">
+        <is>
+          <t>2020 MAR 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>9/13/2019</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>SPE5EJ-19-V-7054</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>$156.00</t>
+        </is>
+      </c>
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>5330010396656</t>
+        </is>
+      </c>
+      <c r="F357" t="inlineStr">
+        <is>
+          <t>GASKET</t>
+        </is>
+      </c>
+      <c r="G357" t="inlineStr">
+        <is>
+          <t>Cameron</t>
+        </is>
+      </c>
+      <c r="H357" t="inlineStr">
+        <is>
+          <t>S888.0016Z</t>
+        </is>
+      </c>
+      <c r="I357" t="inlineStr">
+        <is>
+          <t>M31</t>
+        </is>
+      </c>
+      <c r="J357" t="inlineStr">
+        <is>
+          <t>2020 FEB 20</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
normal day / manual update
</commit_message>
<xml_diff>
--- a/Contract_WIP.xlsx
+++ b/Contract_WIP.xlsx
@@ -327,13 +327,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J361"/>
+  <dimension ref="A1:J371"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A271" workbookViewId="0">
       <selection activeCell="G292" sqref="G292"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="13.7109375"/>
     <col bestFit="1" customWidth="1" max="2" min="2" width="17.7109375"/>
@@ -19101,6 +19101,526 @@
         </is>
       </c>
     </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>9/19/2019</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>SPE7M1-19-V-057Q</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>$2,639.00</t>
+        </is>
+      </c>
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>5935015360017</t>
+        </is>
+      </c>
+      <c r="F362" t="inlineStr">
+        <is>
+          <t>DUMMY CONNECTOR,RECEPTACLE</t>
+        </is>
+      </c>
+      <c r="G362" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H362" t="inlineStr">
+        <is>
+          <t>650HS058NF25</t>
+        </is>
+      </c>
+      <c r="I362" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J362" t="inlineStr">
+        <is>
+          <t>2020 MAR 17</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>9/12/2019</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>SPE7M5-19-V-116M</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>$1,915.00</t>
+        </is>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>5935016512754</t>
+        </is>
+      </c>
+      <c r="F363" t="inlineStr">
+        <is>
+          <t>BACKSHELL,ELECTRICA</t>
+        </is>
+      </c>
+      <c r="G363" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H363" t="inlineStr">
+        <is>
+          <t>443AS024NF1404-3S</t>
+        </is>
+      </c>
+      <c r="I363" t="inlineStr">
+        <is>
+          <t>M31</t>
+        </is>
+      </c>
+      <c r="J363" t="inlineStr">
+        <is>
+          <t>2020 MAR 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>9/12/2019</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>SPE7M1-19-V-046H</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>$849.45</t>
+        </is>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>5935014667112</t>
+        </is>
+      </c>
+      <c r="F364" t="inlineStr">
+        <is>
+          <t>SHELL,ELECTRICAL CO</t>
+        </is>
+      </c>
+      <c r="G364" t="inlineStr">
+        <is>
+          <t>Kern</t>
+        </is>
+      </c>
+      <c r="H364" t="inlineStr">
+        <is>
+          <t>BAT86-19W07C</t>
+        </is>
+      </c>
+      <c r="I364" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J364" t="inlineStr">
+        <is>
+          <t>2020 FEB 19</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>9/12/2019</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>SPE7M5-19-V-116S</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D365" t="inlineStr">
+        <is>
+          <t>$805.20</t>
+        </is>
+      </c>
+      <c r="E365" t="inlineStr">
+        <is>
+          <t>5935015754171</t>
+        </is>
+      </c>
+      <c r="F365" t="inlineStr">
+        <is>
+          <t>COVER,ELECTRICAL CONNECTOR</t>
+        </is>
+      </c>
+      <c r="G365" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H365" t="inlineStr">
+        <is>
+          <t>660-008NF18F6-12</t>
+        </is>
+      </c>
+      <c r="I365" t="inlineStr">
+        <is>
+          <t>ZZ</t>
+        </is>
+      </c>
+      <c r="J365" t="inlineStr">
+        <is>
+          <t>2020 MAR 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>9/12/2019</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>SPE7M5-19-V-116T</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>$1,643.05</t>
+        </is>
+      </c>
+      <c r="E366" t="inlineStr">
+        <is>
+          <t>5935016499431</t>
+        </is>
+      </c>
+      <c r="F366" t="inlineStr">
+        <is>
+          <t>BACKSHELL,ELECTRICA</t>
+        </is>
+      </c>
+      <c r="G366" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H366" t="inlineStr">
+        <is>
+          <t>440AS156NF2216-16-4</t>
+        </is>
+      </c>
+      <c r="I366" t="inlineStr">
+        <is>
+          <t>M41</t>
+        </is>
+      </c>
+      <c r="J366" t="inlineStr">
+        <is>
+          <t>2020 MAR 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>9/12/2019</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>SPE7M5-19-V-115D</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>146</t>
+        </is>
+      </c>
+      <c r="D367" t="inlineStr">
+        <is>
+          <t>$7,089.76</t>
+        </is>
+      </c>
+      <c r="E367" t="inlineStr">
+        <is>
+          <t>5935015812863</t>
+        </is>
+      </c>
+      <c r="F367" t="inlineStr">
+        <is>
+          <t>BACKSHELL,ELECTRICAL CONNECTOR</t>
+        </is>
+      </c>
+      <c r="G367" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H367" t="inlineStr">
+        <is>
+          <t>447HS105NF0901K</t>
+        </is>
+      </c>
+      <c r="I367" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J367" t="inlineStr">
+        <is>
+          <t>2020 MAR 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>9/12/2019</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>SPE7M5-19-V-116K</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D368" t="inlineStr">
+        <is>
+          <t>$1,244.28</t>
+        </is>
+      </c>
+      <c r="E368" t="inlineStr">
+        <is>
+          <t>5935015754188</t>
+        </is>
+      </c>
+      <c r="F368" t="inlineStr">
+        <is>
+          <t>COVER,ELECTRICAL CO</t>
+        </is>
+      </c>
+      <c r="G368" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H368" t="inlineStr">
+        <is>
+          <t>660-008NF22F6-16</t>
+        </is>
+      </c>
+      <c r="I368" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J368" t="inlineStr">
+        <is>
+          <t>2020 MAR 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>9/20/2019</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>SPE5E3-19-V-061E</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="D369" t="inlineStr">
+        <is>
+          <t>$332.28</t>
+        </is>
+      </c>
+      <c r="E369" t="inlineStr">
+        <is>
+          <t>5330015847794</t>
+        </is>
+      </c>
+      <c r="F369" t="inlineStr">
+        <is>
+          <t>GASKET</t>
+        </is>
+      </c>
+      <c r="G369" t="inlineStr">
+        <is>
+          <t>Cameron</t>
+        </is>
+      </c>
+      <c r="H369" t="inlineStr">
+        <is>
+          <t>9A.0199.0027C</t>
+        </is>
+      </c>
+      <c r="I369" t="inlineStr">
+        <is>
+          <t>M10</t>
+        </is>
+      </c>
+      <c r="J369" t="inlineStr">
+        <is>
+          <t>2020 FEB 27</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>9/20/2019</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>SPE5EJ-19-V-7230</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D370" t="inlineStr">
+        <is>
+          <t>$290.30</t>
+        </is>
+      </c>
+      <c r="E370" t="inlineStr">
+        <is>
+          <t>5330010771949</t>
+        </is>
+      </c>
+      <c r="F370" t="inlineStr">
+        <is>
+          <t>GASKET</t>
+        </is>
+      </c>
+      <c r="G370" t="inlineStr">
+        <is>
+          <t>Munters</t>
+        </is>
+      </c>
+      <c r="H370" t="inlineStr">
+        <is>
+          <t>C60508-01</t>
+        </is>
+      </c>
+      <c r="I370" t="inlineStr">
+        <is>
+          <t>M31</t>
+        </is>
+      </c>
+      <c r="J370" t="inlineStr">
+        <is>
+          <t>2020 FEB 27</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>9/20/2019</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>SPE7M8-19-P-3507</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D371" t="inlineStr">
+        <is>
+          <t>$8,610.00</t>
+        </is>
+      </c>
+      <c r="E371" t="inlineStr">
+        <is>
+          <t>5930011263228</t>
+        </is>
+      </c>
+      <c r="F371" t="inlineStr">
+        <is>
+          <t>SWITCH ASSEMBLY</t>
+        </is>
+      </c>
+      <c r="G371" t="inlineStr">
+        <is>
+          <t>Cole</t>
+        </is>
+      </c>
+      <c r="H371" t="inlineStr">
+        <is>
+          <t>3600-3623</t>
+        </is>
+      </c>
+      <c r="I371" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J371" t="inlineStr">
+        <is>
+          <t>2020 MAR 16</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
manual update / bug fixes
</commit_message>
<xml_diff>
--- a/Contract_WIP.xlsx
+++ b/Contract_WIP.xlsx
@@ -327,13 +327,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J381"/>
+  <dimension ref="A1:J383"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A271" workbookViewId="0">
       <selection activeCell="G292" sqref="G292"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="13.7109375"/>
     <col bestFit="1" customWidth="1" max="2" min="2" width="17.7109375"/>
@@ -20141,6 +20141,110 @@
         </is>
       </c>
     </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>9/27/2019</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>SPE7MC-19-V-085X</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>$4,704.00</t>
+        </is>
+      </c>
+      <c r="E382" t="inlineStr">
+        <is>
+          <t>5935010578732</t>
+        </is>
+      </c>
+      <c r="F382" t="inlineStr">
+        <is>
+          <t>BACKSHELL,ELECTRICA</t>
+        </is>
+      </c>
+      <c r="G382" t="inlineStr">
+        <is>
+          <t>Glenair</t>
+        </is>
+      </c>
+      <c r="H382" t="inlineStr">
+        <is>
+          <t>G5796N2820MN</t>
+        </is>
+      </c>
+      <c r="I382" t="inlineStr">
+        <is>
+          <t>CP</t>
+        </is>
+      </c>
+      <c r="J382" t="inlineStr">
+        <is>
+          <t>2020 MAR 25</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>9/27/2019</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>SPE4A6-19-P-P489</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>$4,737.88</t>
+        </is>
+      </c>
+      <c r="E383" t="inlineStr">
+        <is>
+          <t>6685014522074</t>
+        </is>
+      </c>
+      <c r="F383" t="inlineStr">
+        <is>
+          <t>GAGE, DIFFERENTIAL, DIAL INDICATING</t>
+        </is>
+      </c>
+      <c r="G383" t="inlineStr">
+        <is>
+          <t>Cameron</t>
+        </is>
+      </c>
+      <c r="H383" t="inlineStr">
+        <is>
+          <t>19BCXXX0X30E1BXAXX05</t>
+        </is>
+      </c>
+      <c r="I383" t="inlineStr">
+        <is>
+          <t>M10</t>
+        </is>
+      </c>
+      <c r="J383" t="inlineStr">
+        <is>
+          <t>2020 MAR 16</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>